<commit_message>
Atualização do Documento de Acompanhamento da OS 4721 e do Relatório de Ciclo de Testes.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/05_ORDEM_SERVICO/01_OS4721/02_TESTES/OS 4721 - Relatório de Ciclo de Testes.xlsx
+++ b/00_GESTAO_GERAL/05_ORDEM_SERVICO/01_OS4721/02_TESTES/OS 4721 - Relatório de Ciclo de Testes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marqu\Desktop\Teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\MeusArqs-Consultorias\CIAT-Panama\Ciclos de Teste\TAG 1.2.2\Relatório de Teste\Versão 2 - atualização do JP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -268,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -362,11 +362,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -436,6 +462,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,7 +704,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -731,7 +769,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>261</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1333,10 +1371,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>238</c:v>
@@ -2392,7 +2430,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -2556,13 +2594,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>261</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>238</c:v>
@@ -2952,7 +2990,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3083,7 +3121,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
@@ -3092,7 +3130,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7</c:v>
@@ -3326,16 +3364,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8</c:v>
@@ -5855,7 +5893,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M50"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6111,7 +6149,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6119,6 +6157,7 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -6187,17 +6226,18 @@
       <c r="H35" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="J35" s="27"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="4">
-        <v>13</v>
+        <f>C36+D36</f>
+        <v>7</v>
       </c>
       <c r="C36" s="4">
         <v>3</v>
@@ -6217,25 +6257,24 @@
       <c r="H36" s="10">
         <v>152</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="28">
         <v>0</v>
       </c>
-      <c r="J36" s="10"/>
+      <c r="J36" s="29"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="4">
-        <f>SUM(C37:E37)</f>
-        <v>261</v>
+      <c r="B37" s="10">
+        <f>C37+D37</f>
+        <v>20</v>
       </c>
       <c r="C37" s="4">
-        <f>'V 1.2.2'!C46</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E37" s="10">
         <v>238</v>
@@ -6249,10 +6288,10 @@
       <c r="H37" s="10">
         <v>4</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="28">
         <v>68</v>
       </c>
-      <c r="J37" s="10"/>
+      <c r="J37" s="29"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
@@ -6263,12 +6302,16 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A1:P2"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="79" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -6285,7 +6328,7 @@
   <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6401,13 +6444,13 @@
       </c>
       <c r="B38" s="10">
         <f t="shared" ref="B38:B45" si="0">SUM(C38:D38)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" s="4">
         <v>2</v>
       </c>
       <c r="D38" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -6431,10 +6474,10 @@
       </c>
       <c r="B40" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="4">
         <v>0</v>
@@ -6446,13 +6489,13 @@
       </c>
       <c r="B41" s="10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
       </c>
       <c r="D41" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -6521,15 +6564,15 @@
       </c>
       <c r="B46" s="7">
         <f>SUM(B37:B45)</f>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C46" s="7">
         <f>SUM(C37:C45)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46" s="7">
         <f t="shared" ref="D46" si="1">SUM(D37:D45)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>